<commit_message>
update timeline, upload interview responses
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinloh/Desktop/DSA3101/dsa3101-2220-03-airline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanda/Desktop/dsa3101_datasciprac/project/dsa3101-2220-03-airline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7864013-54E5-8741-974A-7F8AF564FC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BD378C-39D5-5546-866A-BCBFFE394776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="23740" windowHeight="16940" xr2:uid="{0CF4B2C0-5CF5-7944-9B83-2A2054250278}"/>
+    <workbookView xWindow="9500" yWindow="500" windowWidth="18920" windowHeight="16940" xr2:uid="{0CF4B2C0-5CF5-7944-9B83-2A2054250278}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Week 9</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Finish creating models draft 1 before meeting</t>
   </si>
   <si>
-    <t>Implement more flight data viz options before meeting</t>
-  </si>
-  <si>
     <t>Modelling</t>
   </si>
   <si>
@@ -99,6 +96,21 @@
   </si>
   <si>
     <t>Viz plots</t>
+  </si>
+  <si>
+    <t>Consolidate all interview responses for backend</t>
+  </si>
+  <si>
+    <t>Implement testing flight data viz with Plotly</t>
+  </si>
+  <si>
+    <t>Get model and data from backend</t>
+  </si>
+  <si>
+    <t>Implement skeleton interactive viz based on model and actual data</t>
+  </si>
+  <si>
+    <t>Integrate frontend, backend during meeting</t>
   </si>
 </sst>
 </file>
@@ -435,6 +447,42 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,42 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,10 +845,10 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,46 +861,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="33" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="32" t="s">
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="34"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="46"/>
       <c r="X1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="42"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="54"/>
       <c r="C2" s="5">
         <v>44998</v>
       </c>
@@ -956,8 +968,8 @@
         <v>45019</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="13" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:24" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -972,7 +984,9 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="H3" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="I3" s="12"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
@@ -990,8 +1004,8 @@
       <c r="W3" s="12"/>
       <c r="X3" s="11"/>
     </row>
-    <row r="4" spans="1:24" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+    <row r="4" spans="1:24" s="18" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A4" s="48"/>
       <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
@@ -1002,15 +1016,19 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="17"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="L4" s="16" t="s">
+        <v>22</v>
+      </c>
       <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="N4" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="O4" s="16"/>
       <c r="P4" s="16"/>
       <c r="Q4" s="15"/>
@@ -1022,8 +1040,8 @@
       <c r="W4" s="17"/>
       <c r="X4" s="16"/>
     </row>
-    <row r="5" spans="1:24" s="23" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+    <row r="5" spans="1:24" s="23" customFormat="1" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
       <c r="B5" s="19" t="s">
         <v>7</v>
       </c>
@@ -1038,7 +1056,9 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
+      <c r="N5" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="20"/>
@@ -1051,7 +1071,7 @@
       <c r="X5" s="21"/>
     </row>
     <row r="6" spans="1:24" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="50" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="24"/>
@@ -1083,9 +1103,9 @@
       <c r="X6" s="26"/>
     </row>
     <row r="7" spans="1:24" s="18" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="30"/>
@@ -1113,90 +1133,92 @@
       <c r="X7" s="30"/>
     </row>
     <row r="8" spans="1:24" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
-      <c r="B8" s="47" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="48"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="35"/>
     </row>
     <row r="9" spans="1:24" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
-      <c r="B9" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="55"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="42"/>
     </row>
-    <row r="10" spans="1:24" s="18" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="49" t="s">
+    <row r="10" spans="1:24" s="18" customFormat="1" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="51"/>
-      <c r="T10" s="51"/>
-      <c r="U10" s="51"/>
-      <c r="V10" s="51"/>
-      <c r="W10" s="52"/>
-      <c r="X10" s="51"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>